<commit_message>
Updated to last LGPL licensed EPPlus. Update to net 4.7.2 and tested on Simio 14.240
</commit_message>
<xml_diff>
--- a/Data/ImportObjectsLinksVertices.xlsx
+++ b/Data/ImportObjectsLinksVertices.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OldOneDrive\Everything\Development\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\(svn azure)\SimioCloud\API\Examples2019\ImportObjectsFromExcelUsingEPPlus\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3197C34-FD92-48CE-833B-6A5544078759}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11280" yWindow="60" windowWidth="8160" windowHeight="9480"/>
+    <workbookView xWindow="30990" yWindow="2295" windowWidth="21810" windowHeight="15105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Objects1" sheetId="4" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="52">
   <si>
     <t>X</t>
   </si>
@@ -174,12 +175,15 @@
   </si>
   <si>
     <t>1 Row;AssignmentsOnEnteringStateVariableName;ModelEntity.Picture~AssignmentsOnEnteringNewValue;1</t>
+  </si>
+  <si>
+    <t>Always</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -243,10 +247,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -590,84 +593,84 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q21" sqref="Q21"/>
+      <selection pane="bottomLeft" activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.25" customWidth="1"/>
-    <col min="2" max="2" width="17.125" customWidth="1"/>
-    <col min="3" max="3" width="6.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="7.75" customWidth="1"/>
-    <col min="8" max="8" width="8.875" customWidth="1"/>
-    <col min="9" max="9" width="14.25" customWidth="1"/>
-    <col min="10" max="10" width="20.375" customWidth="1"/>
-    <col min="11" max="12" width="18.25" customWidth="1"/>
-    <col min="13" max="13" width="11.125" customWidth="1"/>
-    <col min="14" max="14" width="11.25" customWidth="1"/>
-    <col min="15" max="15" width="10.375" customWidth="1"/>
-    <col min="16" max="16" width="19.125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="69.875" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" customWidth="1"/>
+    <col min="11" max="12" width="18.28515625" customWidth="1"/>
+    <col min="13" max="13" width="11.140625" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" customWidth="1"/>
+    <col min="15" max="15" width="10.42578125" customWidth="1"/>
+    <col min="16" max="16" width="9.42578125" customWidth="1"/>
+    <col min="17" max="17" width="69.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="2" t="s">
         <v>48</v>
       </c>
     </row>
@@ -753,7 +756,7 @@
       <c r="P5">
         <v>2</v>
       </c>
-      <c r="Q5" s="2" t="s">
+      <c r="Q5" t="s">
         <v>50</v>
       </c>
     </row>
@@ -790,8 +793,8 @@
       <c r="E7">
         <v>-10</v>
       </c>
-      <c r="K7" t="b">
-        <v>1</v>
+      <c r="K7" t="s">
+        <v>51</v>
       </c>
       <c r="L7" t="s">
         <v>28</v>
@@ -813,22 +816,22 @@
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="K8" t="b">
-        <v>1</v>
+      <c r="K8" t="s">
+        <v>51</v>
       </c>
       <c r="L8" t="s">
         <v>28</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:XFD27">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:XFD27">
     <sortCondition ref="C2:C27"/>
     <sortCondition ref="E2:E27"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="A7" r:id="rId1" display="Output@Source1"/>
-    <hyperlink ref="A8" r:id="rId2" display="Output@Source1"/>
-    <hyperlink ref="B8" r:id="rId3"/>
+    <hyperlink ref="A7" r:id="rId1" display="Output@Source1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="A8" r:id="rId2" display="Output@Source1" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B8" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId4"/>
@@ -836,7 +839,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -844,17 +847,16 @@
       <selection pane="bottomLeft" activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="10.25" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="15.75" style="2" customWidth="1"/>
-    <col min="5" max="6" width="13.75" style="2" customWidth="1"/>
-    <col min="7" max="7" width="14" style="2" customWidth="1"/>
-    <col min="8" max="8" width="12.75" style="2" customWidth="1"/>
-    <col min="9" max="9" width="13.875" style="2" customWidth="1"/>
-    <col min="10" max="16384" width="8.875" style="2"/>
+    <col min="1" max="1" width="9.5703125" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -887,146 +889,146 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>25</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" t="s">
         <v>43</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" t="s">
         <v>36</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="D2" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
-    <hyperlink ref="D4" r:id="rId4"/>
-    <hyperlink ref="C3" r:id="rId5"/>
-    <hyperlink ref="D3" r:id="rId6"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="D4" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="C3" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="D3" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2">
         <v>-1</v>
       </c>
-      <c r="C2" s="2">
-        <v>0</v>
-      </c>
-      <c r="D2" s="2">
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
         <v>-6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" s="2">
-        <v>0</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
         <v>-6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
         <v>4</v>
       </c>
-      <c r="C4" s="2">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
         <v>-3</v>
       </c>
     </row>

</xml_diff>